<commit_message>
update ExcelHelper, add DataProvider
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata/CRM.xlsx
+++ b/src/main/resources/testdata/CRM.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Source\SeleniumFramework\src\main\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BB9CCDA-770F-4640-8F82-CD1547F7FF6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E1D7475-EF5D-41AA-AFDC-28BA46525943}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6585" yWindow="5535" windowWidth="38700" windowHeight="15345" xr2:uid="{9190CBA4-F86D-4037-A35E-ED0FA62C21A4}"/>
+    <workbookView xWindow="6585" yWindow="5535" windowWidth="38700" windowHeight="15345" activeTab="1" xr2:uid="{9190CBA4-F86D-4037-A35E-ED0FA62C21A4}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Signin" sheetId="1" r:id="rId1"/>
+    <sheet name="SigninCustom" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,12 +35,30 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
-  <si>
-    <t>USERNAME</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="8">
   <si>
     <t>PASSWORD</t>
+  </si>
+  <si>
+    <t>EMAIL</t>
+  </si>
+  <si>
+    <t>admin@demo.com</t>
+  </si>
+  <si>
+    <t>riseDemo</t>
+  </si>
+  <si>
+    <t>admin2@demo.com</t>
+  </si>
+  <si>
+    <t>RESULT</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>client@demo.com</t>
   </si>
 </sst>
 </file>
@@ -75,8 +94,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -391,27 +411,147 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD5EFDBF-2ED4-49CF-8DFF-DFBC655876DA}">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.28515625" customWidth="1"/>
     <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A3" r:id="rId1" xr:uid="{F3037AF4-B7EE-4990-9A1A-940972B187BD}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FAB4695-8788-4649-959C-A08BAA7A7A14}">
+  <dimension ref="A1:C7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="30.28515625" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C7" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>